<commit_message>
commit avant gestion des scénarios
</commit_message>
<xml_diff>
--- a/data/triangle_v5.xlsx
+++ b/data/triangle_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Chouette\Python\AssembleurTriangles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5119E85B-6DD4-452B-9E78-4D0C68BCA7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E1C5E9A5-FDB4-4222-9CEA-EB020C114678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="10350" windowWidth="29040" windowHeight="15840" xr2:uid="{0502679B-B5E7-4C24-BB1F-BD2412F138B2}"/>
+    <workbookView xWindow="-28920" yWindow="10350" windowWidth="29040" windowHeight="15840" xr2:uid="{784FA908-1E02-43A4-A21A-BF3D95BA3A1D}"/>
   </bookViews>
   <sheets>
     <sheet name="triangle_v5" sheetId="1" r:id="rId1"/>
@@ -151,22 +151,22 @@
     <t>Pertuis d'Antioche</t>
   </si>
   <si>
-    <t>18.98</t>
-  </si>
-  <si>
-    <t>57.48</t>
-  </si>
-  <si>
-    <t>103.54</t>
+    <t>18.27</t>
+  </si>
+  <si>
+    <t>57.87</t>
+  </si>
+  <si>
+    <t>103.86</t>
   </si>
   <si>
     <t>346.27</t>
   </si>
   <si>
-    <t>300.23</t>
-  </si>
-  <si>
-    <t>115.69</t>
+    <t>301.97</t>
+  </si>
+  <si>
+    <t>111.63</t>
   </si>
   <si>
     <t>Beaugency</t>
@@ -1572,7 +1572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F859EAE-9F65-43C9-921E-6D1F23EAB6C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B6E617-710A-4B71-AFEA-DA91DDF70D5E}">
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1581,8 +1581,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="10.3984375" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="1" max="11" width="16.9296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -2331,28 +2330,28 @@
         <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E22" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="F22" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G22" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H22" t="s">
         <v>148</v>
       </c>
       <c r="I22" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="J22" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="K22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -2366,28 +2365,28 @@
         <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G23" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H23" t="s">
         <v>148</v>
       </c>
       <c r="I23" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K23" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">

</xml_diff>